<commit_message>
Completed i.) -> vii.) data analysis
</commit_message>
<xml_diff>
--- a/Lab 04 Report/src/Lab 4 Calibration Data.xlsx
+++ b/Lab 04 Report/src/Lab 4 Calibration Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcmehrtens/Documents/Aerospace Undergrad/07 - Spring 2023/AER E 322/AER-E-322-lab-04/Lab 04 Report/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97D8AA51-5ABE-4E56-ABE3-C477C7FF6C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C358E5-782E-E347-B108-9B0C26CFF60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{5E372F63-C1CD-4A76-880F-6518DF0419E1}"/>
+    <workbookView xWindow="40960" yWindow="9240" windowWidth="10240" windowHeight="10920" xr2:uid="{5E372F63-C1CD-4A76-880F-6518DF0419E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,12 +399,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>89</v>
       </c>
@@ -426,7 +431,7 @@
         <v>6.0999999999999997E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>169</v>
       </c>
@@ -437,7 +442,7 @@
         <v>1.23E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>245</v>
       </c>
@@ -448,7 +453,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>310</v>
       </c>
@@ -459,7 +464,7 @@
         <v>2.4599999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>372</v>
       </c>
@@ -470,7 +475,7 @@
         <v>3.0799999999999998E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>443</v>
       </c>

</xml_diff>